<commit_message>
hyperparameter search for DNA updated
</commit_message>
<xml_diff>
--- a/hyperparameter search/NO2/hyperparameter_optimization_results.xlsx
+++ b/hyperparameter search/NO2/hyperparameter_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikodemas\Desktop\monikai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478B5EDE-2B94-4510-9BDB-2E3C291D0349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92D2AED-F657-476A-9B97-D80354BA3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{AD279D57-B0C1-4544-A24A-7AD6676E0DF7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{AD279D57-B0C1-4544-A24A-7AD6676E0DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="lstm" sheetId="2" state="hidden" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="dna" sheetId="1" state="hidden" r:id="rId3"/>
     <sheet name="dna (2)" sheetId="4" r:id="rId4"/>
     <sheet name="lstm dates" sheetId="5" r:id="rId5"/>
-    <sheet name="na dates" sheetId="6" r:id="rId6"/>
+    <sheet name="dna dates" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'dna dates'!$A$2:$B$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'lstm dates'!$A$2:$B$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'na dates'!$A$2:$B$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="361">
   <si>
     <t>SEQUENCE LENGTH</t>
   </si>
@@ -937,6 +937,195 @@
   </si>
   <si>
     <t>average time per station</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:24</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:02:58</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:55:29</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:01:50</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:55:33</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:07:03</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:08:44</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:03:10</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:01</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:23:08</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:08:31</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:12</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:20:26</t>
+  </si>
+  <si>
+    <t>30/08/2021 14:47:04</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:02</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:14:30</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:19:16</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:53:25</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:07:55</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:25:26</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:50:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:57:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:28:42</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:33:38</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:23:47</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:37:30</t>
+  </si>
+  <si>
+    <t>30/08/2021 18:12:18</t>
+  </si>
+  <si>
+    <t>30/08/2021 18:33:56</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:54:46</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:10:42</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:33:36</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:56:10</t>
+  </si>
+  <si>
+    <t>30/08/2021 18:44:17</t>
+  </si>
+  <si>
+    <t>30/08/2021 18:34:26</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:05:27</t>
+  </si>
+  <si>
+    <t>30/08/2021 19:02:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:54:32</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:49:03</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:07:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 19:17:58</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:59:15</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:03:49</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:05:30</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:54:18</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:07:45</t>
+  </si>
+  <si>
+    <t>30/08/2021 20:00:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:53:57</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:37:47</t>
+  </si>
+  <si>
+    <t>30/08/2021 21:30:07</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:49:38</t>
+  </si>
+  <si>
+    <t>30/08/2021 16:26:27</t>
+  </si>
+  <si>
+    <t>30/08/2021 13:00:00</t>
+  </si>
+  <si>
+    <t>30/08/2021 18:46:27</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:57:32</t>
+  </si>
+  <si>
+    <t>30/08/2021 21:01:36</t>
+  </si>
+  <si>
+    <t>30/08/2021 21:25:41</t>
+  </si>
+  <si>
+    <t>30/08/2021 17:11:34</t>
+  </si>
+  <si>
+    <t>30/08/2021 15:06:54</t>
+  </si>
+  <si>
+    <t>30/08/2021 20:48:02</t>
+  </si>
+  <si>
+    <t>30/08/2021 20:29:03</t>
+  </si>
+  <si>
+    <t>30/08/2021 12:58:11</t>
+  </si>
+  <si>
+    <t>30/08/2021 19:01:02</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1134,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1006,7 +1195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1016,11 +1205,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3320,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF6F320-061F-44F2-A88D-51287D47366E}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5334,7 +5526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71510-37F4-423C-AE36-33C61C25993D}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -7260,67 +7452,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60EBA90-8DF9-4DB0-B3AB-C5B318E79415}">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="15" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -7346,756 +7547,760 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>7435.5829763412403</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="6">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="F3" s="1">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16">
+        <v>4114.3090088367398</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" s="16">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="F3" s="8">
         <v>40</v>
       </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
-        <v>40</v>
-      </c>
-      <c r="K3" s="1">
-        <v>10</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.326610207557678</v>
+      <c r="G3" s="8">
+        <v>35</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>20</v>
+      </c>
+      <c r="J3" s="8">
+        <v>20</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="16">
+        <v>0.24976783990859899</v>
       </c>
       <c r="O3" s="1">
         <f>SUM(B3:B11,B15:B23,B27:B35,B39:B47,B51:B59)</f>
-        <v>433907.88079881546</v>
+        <v>638926.71762800065</v>
       </c>
       <c r="P3" s="1">
         <f>O3/3600</f>
-        <v>120.52996688855985</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>255</v>
+        <v>177.47964378555574</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="S3" s="13">
-        <v>0.2598611111111111</v>
+        <v>0.35844907407407406</v>
       </c>
       <c r="T3" s="1">
-        <f>6+((14*60+12)/3600)</f>
-        <v>6.2366666666666664</v>
+        <f>8+(36*60 + 10)/3600</f>
+        <v>8.6027777777777779</v>
       </c>
       <c r="U3" s="1">
         <f>P3/4</f>
-        <v>30.132491722139964</v>
+        <v>44.369910946388934</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="A4" s="8">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
-        <v>8319.2666363716107</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="6">
-        <v>6.3499999999999997E-3</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="B4" s="16">
+        <v>8947.5812113284992</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4" s="16">
+        <v>4.2500000000000003E-3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="16">
+        <v>0.24429510533809601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16">
+        <v>12314.4837551116</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="F5" s="8">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>20</v>
+      </c>
+      <c r="J5" s="8">
+        <v>55</v>
+      </c>
+      <c r="K5" s="8">
+        <v>10</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0.24399603903293601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16">
+        <v>14579.2368552684</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>50</v>
+      </c>
+      <c r="G6" s="8">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>45</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0.243764042854309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7">
+        <v>19096.355388164498</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9.5E-4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>50</v>
+      </c>
+      <c r="G7" s="4">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
         <v>60</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0.24340723454952201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>16</v>
+      </c>
+      <c r="B8" s="16">
+        <v>20886.4339394569</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>55</v>
+      </c>
+      <c r="G8" s="8">
+        <v>55</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8">
+        <v>15</v>
+      </c>
+      <c r="J8" s="8">
+        <v>35</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0.243860304355621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>19</v>
+      </c>
+      <c r="B9" s="16">
+        <v>14673.742902517301</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2.0500000000000002E-3</v>
+      </c>
+      <c r="F9" s="8">
+        <v>50</v>
+      </c>
+      <c r="G9" s="8">
+        <v>50</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.244215622544288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>22</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>25</v>
+      </c>
+      <c r="B11" s="16">
+        <v>30488.421541929201</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E11" s="16">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>45</v>
+      </c>
+      <c r="G11" s="8">
+        <v>25</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0.243627294898033</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="8">
+        <v>1</v>
+      </c>
+      <c r="B15" s="16">
+        <v>3980.8556678295099</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E15" s="16">
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>45</v>
+      </c>
+      <c r="G15" s="8">
+        <v>20</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8">
+        <v>10</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="16">
+        <v>7.4658961296081499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="8">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8">
+        <v>8070.0308098793003</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16" s="8">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="F16" s="8">
+        <v>45</v>
+      </c>
+      <c r="G16" s="8">
+        <v>35</v>
+      </c>
+      <c r="H16" s="8">
+        <v>2</v>
+      </c>
+      <c r="I16" s="8">
+        <v>10</v>
+      </c>
+      <c r="J16" s="8">
+        <v>10</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="8">
+        <v>7.44374179840087</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="8">
+        <v>7</v>
+      </c>
+      <c r="B17" s="16">
+        <v>10763.291496515199</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" s="16">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="F17" s="8">
+        <v>45</v>
+      </c>
+      <c r="G17" s="8">
+        <v>45</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="16">
+        <v>7.43542432785034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <v>10</v>
+      </c>
+      <c r="B18" s="16">
+        <v>16480.827034473401</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1.9499999999999999E-3</v>
+      </c>
+      <c r="F18" s="8">
         <v>60</v>
       </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="G18" s="8">
+        <v>55</v>
+      </c>
+      <c r="H18" s="8">
+        <v>2</v>
+      </c>
+      <c r="I18" s="8">
         <v>40</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.32136899232864302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6919.3482072353299</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="6">
-        <v>3.0500000000000002E-3</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="J18" s="8">
+        <v>25</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="16">
+        <v>7.4419250488281197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="8">
+        <v>13</v>
+      </c>
+      <c r="B19" s="16">
+        <v>20394.523804903001</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E19" s="16">
+        <v>2.15E-3</v>
+      </c>
+      <c r="F19" s="8">
+        <v>20</v>
+      </c>
+      <c r="G19" s="8">
         <v>30</v>
       </c>
-      <c r="G5" s="1">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H19" s="8">
+        <v>3</v>
+      </c>
+      <c r="I19" s="8">
         <v>20</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0.31885498762130698</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <v>5076.6360905170404</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E6" s="6">
-        <v>8.6499999999999997E-3</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="J19" s="8">
+        <v>50</v>
+      </c>
+      <c r="K19" s="8">
+        <v>50</v>
+      </c>
+      <c r="L19" s="16">
+        <v>7.4394025802612296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>16</v>
+      </c>
+      <c r="B20" s="7">
+        <v>20296.3885636329</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="F20" s="4">
+        <v>60</v>
+      </c>
+      <c r="G20" s="4">
+        <v>15</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>55</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="7">
+        <v>7.43312215805053</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="16">
+        <v>10128.326180934901</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F21" s="8">
+        <v>45</v>
+      </c>
+      <c r="G21" s="8">
+        <v>55</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="16">
+        <v>7.43790531158447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>22</v>
+      </c>
+      <c r="B22" s="16">
+        <v>14141.1981284618</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="16">
+        <v>2.0500000000000002E-3</v>
+      </c>
+      <c r="F22" s="8">
+        <v>50</v>
+      </c>
+      <c r="G22" s="8">
         <v>30</v>
       </c>
-      <c r="G6" s="1">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0.31941434741020203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6">
-        <v>11518.1880393028</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2.5500000000000002E-3</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8">
+        <v>40</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="16">
+        <v>7.4353895187377903</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>25</v>
+      </c>
+      <c r="B23" s="16">
+        <v>15456.8977196216</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F23" s="8">
+        <v>35</v>
+      </c>
+      <c r="G23" s="8">
+        <v>35</v>
+      </c>
+      <c r="H23" s="8">
+        <v>2</v>
+      </c>
+      <c r="I23" s="8">
+        <v>55</v>
+      </c>
+      <c r="J23" s="8">
         <v>15</v>
       </c>
-      <c r="G7" s="1">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0.31981831789016701</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>16</v>
-      </c>
-      <c r="B8" s="6">
-        <v>13173.3202981948</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E8" s="6">
-        <v>2.8E-3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>35</v>
-      </c>
-      <c r="G8" s="1">
-        <v>40</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>30</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0.31940683722495999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6">
-        <v>9030.2305016517603</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" s="6">
-        <v>2.8E-3</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45</v>
-      </c>
-      <c r="G9" s="1">
-        <v>30</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
-        <v>45</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0.31961712241172702</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>22</v>
-      </c>
-      <c r="B10" s="7">
-        <v>20467.653292894302</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E10" s="4">
-        <v>4.4999999999999999E-4</v>
-      </c>
-      <c r="F10" s="4">
-        <v>45</v>
-      </c>
-      <c r="G10" s="4">
-        <v>40</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2</v>
-      </c>
-      <c r="I10" s="4">
-        <v>45</v>
-      </c>
-      <c r="J10" s="4">
-        <v>25</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="7">
-        <v>0.31700676679611201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6">
-        <v>13899.7411618232</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E11" s="6">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F11" s="1">
-        <v>25</v>
-      </c>
-      <c r="G11" s="1">
-        <v>30</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>30</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0.31973350048065102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2026.1473526954601</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="6">
-        <v>4.45E-3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>25</v>
-      </c>
-      <c r="G15" s="1">
-        <v>15</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1">
-        <v>55</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="6">
-        <v>8.0988426208496094</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6">
-        <v>10250.1005434989</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1.25E-3</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45</v>
-      </c>
-      <c r="G17" s="1">
-        <v>40</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="6">
-        <v>8.0901346206665004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7">
-        <v>11591.589290857301</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E18" s="4">
-        <v>9.0500000000000008E-3</v>
-      </c>
-      <c r="F18" s="4">
-        <v>35</v>
-      </c>
-      <c r="G18" s="4">
-        <v>40</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="7">
-        <v>8.0861120223999006</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>13</v>
-      </c>
-      <c r="B19" s="6">
-        <v>9999.8391633033698</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E19" s="6">
-        <v>2.2499999999999998E-3</v>
-      </c>
-      <c r="F19" s="1">
-        <v>40</v>
-      </c>
-      <c r="G19" s="1">
-        <v>10</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="6">
-        <v>8.0903615951537997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>16</v>
-      </c>
-      <c r="B20" s="6">
-        <v>10192.778708219499</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E20" s="6">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="F20" s="1">
-        <v>15</v>
-      </c>
-      <c r="G20" s="1">
-        <v>50</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" s="6">
-        <v>8.1007137298583896</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="6">
-        <v>18062.934043169</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1.8500000000000001E-3</v>
-      </c>
-      <c r="F21" s="1">
-        <v>30</v>
-      </c>
-      <c r="G21" s="1">
-        <v>25</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="6">
-        <v>8.1008815765380806</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>22</v>
-      </c>
-      <c r="B22" s="6">
-        <v>13308.9522883892</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E22" s="6">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="F22" s="1">
-        <v>50</v>
-      </c>
-      <c r="G22" s="1">
-        <v>35</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" s="6">
-        <v>8.09814453125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>25</v>
-      </c>
-      <c r="B23" s="6">
-        <v>15480.289604425399</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E23" s="6">
-        <v>6.3499999999999997E-3</v>
-      </c>
-      <c r="F23" s="1">
-        <v>40</v>
-      </c>
-      <c r="G23" s="1">
-        <v>55</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="6">
-        <v>8.0959606170654297</v>
+      <c r="K23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="16">
+        <v>7.4336996078491202</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -8148,36 +8353,38 @@
       <c r="A27" s="1">
         <v>1</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>4289.70440983772</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>302</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>27</v>
+        <v>303</v>
+      </c>
+      <c r="E27" s="1">
+        <v>7.8499999999999993E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1">
+        <v>50</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>15</v>
+      </c>
+      <c r="J27" s="1">
+        <v>35</v>
+      </c>
+      <c r="K27" s="1">
+        <v>15</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1.4759873151779099</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -8185,28 +8392,28 @@
         <v>4</v>
       </c>
       <c r="B28" s="6">
-        <v>3528.8522880077298</v>
+        <v>8774.3796985149293</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>132</v>
+        <v>310</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>133</v>
+        <v>311</v>
       </c>
       <c r="E28" s="6">
-        <v>1.8500000000000001E-3</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="F28" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G28" s="1">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>10</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>27</v>
@@ -8215,7 +8422,7 @@
         <v>27</v>
       </c>
       <c r="L28" s="6">
-        <v>1.7151616811752299</v>
+        <v>1.46154856681823</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -8223,37 +8430,37 @@
         <v>7</v>
       </c>
       <c r="B29" s="6">
-        <v>7349.2917242050098</v>
+        <v>11633.4154775142</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>151</v>
+        <v>313</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>155</v>
+        <v>317</v>
       </c>
       <c r="E29" s="6">
-        <v>3.3500000000000001E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="F29" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G29" s="1">
         <v>20</v>
       </c>
       <c r="H29" s="1">
-        <v>2</v>
-      </c>
-      <c r="I29" s="1">
-        <v>55</v>
-      </c>
-      <c r="J29" s="1">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L29" s="6">
-        <v>1.6980997323989799</v>
+        <v>1.4590262174606301</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -8261,75 +8468,75 @@
         <v>10</v>
       </c>
       <c r="B30" s="6">
-        <v>11688.2663297653</v>
+        <v>13176.5782582759</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>173</v>
+        <v>313</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>177</v>
+        <v>322</v>
       </c>
       <c r="E30" s="6">
-        <v>6.4000000000000003E-3</v>
+        <v>2.5500000000000002E-3</v>
       </c>
       <c r="F30" s="1">
+        <v>55</v>
+      </c>
+      <c r="G30" s="1">
+        <v>35</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>30</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="6">
+        <v>1.4603421688079801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>13</v>
+      </c>
+      <c r="B31" s="16">
+        <v>18044.312942504799</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E31" s="8">
+        <v>3.5500000000000002E-3</v>
+      </c>
+      <c r="F31" s="8">
         <v>40</v>
       </c>
-      <c r="G30" s="1">
-        <v>40</v>
-      </c>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
-      <c r="I30" s="1">
-        <v>20</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="6">
-        <v>1.6967130899429299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4">
-        <v>13</v>
-      </c>
-      <c r="B31" s="7">
-        <v>13050.303891420301</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E31" s="4">
-        <v>2.8500000000000001E-3</v>
-      </c>
-      <c r="F31" s="4">
-        <v>35</v>
-      </c>
-      <c r="G31" s="4">
-        <v>40</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="G31" s="8">
+        <v>25</v>
+      </c>
+      <c r="H31" s="8">
         <v>2</v>
       </c>
-      <c r="I31" s="4">
-        <v>10</v>
-      </c>
-      <c r="J31" s="4">
-        <v>10</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L31" s="7">
-        <v>1.6918975114822301</v>
+      <c r="I31" s="8">
+        <v>15</v>
+      </c>
+      <c r="J31" s="8">
+        <v>55</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="16">
+        <v>1.4566076993942201</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
@@ -8337,28 +8544,28 @@
         <v>16</v>
       </c>
       <c r="B32" s="6">
-        <v>18880.218415737101</v>
+        <v>14192.2366096973</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>220</v>
+        <v>333</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>221</v>
+        <v>334</v>
       </c>
       <c r="E32" s="6">
-        <v>5.4000000000000003E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="F32" s="1">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H32" s="1">
         <v>1</v>
       </c>
       <c r="I32" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>27</v>
@@ -8367,7 +8574,7 @@
         <v>27</v>
       </c>
       <c r="L32" s="6">
-        <v>1.70085608959198</v>
+        <v>1.4586379528045601</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
@@ -8375,75 +8582,75 @@
         <v>19</v>
       </c>
       <c r="B33" s="6">
-        <v>10688.886343002299</v>
+        <v>17534.798295259399</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>240</v>
+        <v>343</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>241</v>
+        <v>344</v>
       </c>
       <c r="E33" s="6">
-        <v>1E-3</v>
+        <v>1.75E-3</v>
       </c>
       <c r="F33" s="1">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G33" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H33" s="1">
-        <v>2</v>
-      </c>
-      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="6">
+        <v>1.4573836326599099</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>22</v>
+      </c>
+      <c r="B34" s="7">
+        <v>12750.123835325199</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="E34" s="7">
+        <v>3.3E-3</v>
+      </c>
+      <c r="F34" s="4">
+        <v>20</v>
+      </c>
+      <c r="G34" s="4">
         <v>30</v>
       </c>
-      <c r="J33" s="1">
-        <v>45</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" s="6">
-        <v>1.69819784164428</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>22</v>
-      </c>
-      <c r="B34" s="6">
-        <v>13413.0543458461</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E34" s="6">
-        <v>4.6499999999999996E-3</v>
-      </c>
-      <c r="F34" s="1">
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
+      <c r="I34" s="4">
         <v>40</v>
       </c>
-      <c r="G34" s="1">
-        <v>30</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1</v>
-      </c>
-      <c r="I34" s="1">
-        <v>30</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" s="6">
-        <v>1.7008360624313299</v>
+      <c r="J34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" s="7">
+        <v>1.4541723728179901</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
@@ -8451,37 +8658,37 @@
         <v>25</v>
       </c>
       <c r="B35" s="6">
-        <v>15478.3983545303</v>
+        <v>20467.940044164599</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>269</v>
+        <v>356</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>281</v>
+        <v>357</v>
       </c>
       <c r="E35" s="6">
-        <v>2.8E-3</v>
+        <v>9.1500000000000001E-3</v>
       </c>
       <c r="F35" s="1">
+        <v>50</v>
+      </c>
+      <c r="G35" s="1">
+        <v>25</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>55</v>
+      </c>
+      <c r="J35" s="1">
         <v>40</v>
       </c>
-      <c r="G35" s="1">
-        <v>30</v>
-      </c>
-      <c r="H35" s="1">
-        <v>1</v>
-      </c>
-      <c r="I35" s="1">
-        <v>60</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="K35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L35" s="6">
-        <v>1.6999084949493399</v>
+        <v>1.4544893503189</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
@@ -8535,37 +8742,37 @@
         <v>1</v>
       </c>
       <c r="B39" s="6">
-        <v>5516.9619984626697</v>
+        <v>4483.5541193485196</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>119</v>
+        <v>305</v>
       </c>
       <c r="E39" s="6">
-        <v>2.8E-3</v>
+        <v>2.0500000000000002E-3</v>
       </c>
       <c r="F39" s="1">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="G39" s="1">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J39" s="1">
-        <v>50</v>
-      </c>
-      <c r="K39" s="1">
-        <v>35</v>
+        <v>55</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="L39" s="6">
-        <v>0.76370567083358698</v>
+        <v>0.494687110185623</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -8573,37 +8780,37 @@
         <v>4</v>
       </c>
       <c r="B40" s="6">
-        <v>3336.1776289939799</v>
+        <v>6772.3427019119199</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>137</v>
+        <v>310</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>138</v>
+        <v>312</v>
       </c>
       <c r="E40" s="6">
-        <v>5.0499999999999998E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="F40" s="1">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G40" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H40" s="1">
-        <v>3</v>
-      </c>
-      <c r="I40" s="1">
-        <v>50</v>
-      </c>
-      <c r="J40" s="1">
-        <v>25</v>
-      </c>
-      <c r="K40" s="1">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="L40" s="6">
-        <v>0.76637917757034302</v>
+        <v>0.49130362272262501</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
@@ -8611,37 +8818,37 @@
         <v>7</v>
       </c>
       <c r="B41" s="6">
-        <v>10492.353997230501</v>
+        <v>12684.584385156601</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>151</v>
+        <v>313</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>159</v>
+        <v>318</v>
       </c>
       <c r="E41" s="6">
-        <v>7.9000000000000008E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="F41" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G41" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H41" s="1">
         <v>2</v>
       </c>
       <c r="I41" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="J41" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L41" s="6">
-        <v>0.76761311292648304</v>
+        <v>0.49138173460960299</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -8649,37 +8856,37 @@
         <v>10</v>
       </c>
       <c r="B42" s="6">
-        <v>6255.3545970916703</v>
+        <v>16185.488355159699</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>181</v>
+        <v>313</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>182</v>
+        <v>323</v>
       </c>
       <c r="E42" s="6">
-        <v>4.5999999999999999E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F42" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G42" s="1">
+        <v>35</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
         <v>30</v>
       </c>
-      <c r="H42" s="1">
-        <v>2</v>
-      </c>
-      <c r="I42" s="1">
-        <v>40</v>
-      </c>
-      <c r="J42" s="1">
-        <v>25</v>
+      <c r="J42" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L42" s="6">
-        <v>0.75669497251510598</v>
+        <v>0.49044489860534601</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -8687,28 +8894,28 @@
         <v>13</v>
       </c>
       <c r="B43" s="6">
-        <v>5459.7302744388498</v>
+        <v>15401.149209737699</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>202</v>
+        <v>307</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="E43" s="6">
-        <v>1.0499999999999999E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="F43" s="1">
         <v>30</v>
       </c>
       <c r="G43" s="1">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="H43" s="1">
-        <v>0</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>35</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>27</v>
@@ -8717,45 +8924,45 @@
         <v>27</v>
       </c>
       <c r="L43" s="6">
-        <v>0.76672297716140703</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
+        <v>0.49095827341079701</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
         <v>16</v>
       </c>
-      <c r="B44" s="6">
-        <v>11556.8222675323</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E44" s="6">
-        <v>3.8500000000000001E-3</v>
-      </c>
-      <c r="F44" s="1">
-        <v>15</v>
-      </c>
-      <c r="G44" s="1">
-        <v>25</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1">
-        <v>30</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L44" s="6">
-        <v>0.756838619709014</v>
+      <c r="B44" s="7">
+        <v>14070.7537798881</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="7">
+        <v>2.8E-3</v>
+      </c>
+      <c r="F44" s="4">
+        <v>45</v>
+      </c>
+      <c r="G44" s="4">
+        <v>40</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4">
+        <v>20</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="7">
+        <v>0.48988559842109602</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
@@ -8763,75 +8970,75 @@
         <v>19</v>
       </c>
       <c r="B45" s="6">
-        <v>15443.0164005756</v>
+        <v>9830.0533697605097</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>245</v>
+        <v>345</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>246</v>
+        <v>346</v>
       </c>
       <c r="E45" s="6">
-        <v>5.1000000000000004E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="F45" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G45" s="1">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H45" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45" s="1">
-        <v>25</v>
-      </c>
-      <c r="J45" s="1">
-        <v>35</v>
-      </c>
-      <c r="K45" s="1">
         <v>10</v>
       </c>
+      <c r="J45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="L45" s="6">
-        <v>0.76072621345519997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
+        <v>0.49024397134780801</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="8">
         <v>22</v>
       </c>
-      <c r="B46" s="7">
-        <v>9243.1754894256592</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="B46" s="16">
+        <v>20786.595285653999</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E46" s="8">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="F46" s="8">
+        <v>50</v>
+      </c>
+      <c r="G46" s="8">
+        <v>20</v>
+      </c>
+      <c r="H46" s="8">
+        <v>1</v>
+      </c>
+      <c r="I46" s="8">
         <v>30</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E46" s="4">
-        <v>4.3E-3</v>
-      </c>
-      <c r="F46" s="4">
-        <v>40</v>
-      </c>
-      <c r="G46" s="4">
-        <v>55</v>
-      </c>
-      <c r="H46" s="4">
-        <v>2</v>
-      </c>
-      <c r="I46" s="4">
-        <v>35</v>
-      </c>
-      <c r="J46" s="4">
-        <v>45</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L46" s="7">
-        <v>0.75299209356307895</v>
+      <c r="J46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" s="16">
+        <v>0.49056959152221602</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
@@ -8839,19 +9046,19 @@
         <v>25</v>
       </c>
       <c r="B47" s="6">
-        <v>13861.6963689327</v>
+        <v>19277.691771268801</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>269</v>
+        <v>343</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>284</v>
+        <v>358</v>
       </c>
       <c r="E47" s="6">
-        <v>2.4499999999999999E-3</v>
+        <v>2.0500000000000002E-3</v>
       </c>
       <c r="F47" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G47" s="1">
         <v>25</v>
@@ -8860,7 +9067,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>27</v>
@@ -8869,7 +9076,7 @@
         <v>27</v>
       </c>
       <c r="L47" s="6">
-        <v>0.75875079631805398</v>
+        <v>0.490941941738128</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
@@ -8923,28 +9130,28 @@
         <v>1</v>
       </c>
       <c r="B51" s="6">
-        <v>2067.3058514595</v>
+        <v>4149.2110409736597</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>123</v>
+        <v>304</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>124</v>
+        <v>306</v>
       </c>
       <c r="E51" s="6">
-        <v>4.9500000000000004E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="F51" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G51" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H51" s="1">
-        <v>1</v>
-      </c>
-      <c r="I51" s="1">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>27</v>
@@ -8953,7 +9160,7 @@
         <v>27</v>
       </c>
       <c r="L51" s="6">
-        <v>0.37615910172462402</v>
+        <v>0.28089156746864302</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -8961,37 +9168,37 @@
         <v>4</v>
       </c>
       <c r="B52" s="7">
-        <v>2938.5868678092902</v>
+        <v>8428.6952540874408</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>142</v>
+        <v>313</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>143</v>
+        <v>314</v>
       </c>
       <c r="E52" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F52" s="4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G52" s="4">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="H52" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="4">
-        <v>55</v>
-      </c>
-      <c r="J52" s="4">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>27</v>
       </c>
       <c r="L52" s="7">
-        <v>0.36694851517677302</v>
+        <v>0.27592870593070901</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
@@ -8999,16 +9206,16 @@
         <v>7</v>
       </c>
       <c r="B53" s="6">
-        <v>3937.8823742866498</v>
+        <v>10557.9154582023</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>163</v>
+        <v>313</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>164</v>
+        <v>319</v>
       </c>
       <c r="E53" s="6">
-        <v>7.45E-3</v>
+        <v>5.2500000000000003E-3</v>
       </c>
       <c r="F53" s="1">
         <v>40</v>
@@ -9017,19 +9224,19 @@
         <v>30</v>
       </c>
       <c r="H53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" s="1">
-        <v>25</v>
-      </c>
-      <c r="J53" s="1">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L53" s="6">
-        <v>0.37901943922042802</v>
+        <v>0.27629032731056202</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
@@ -9037,19 +9244,19 @@
         <v>10</v>
       </c>
       <c r="B54" s="6">
-        <v>4477.65745949745</v>
+        <v>17007.981338024099</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>186</v>
+        <v>313</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>187</v>
+        <v>324</v>
       </c>
       <c r="E54" s="6">
-        <v>5.0000000000000001E-3</v>
+        <v>7.1500000000000001E-3</v>
       </c>
       <c r="F54" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G54" s="1">
         <v>40</v>
@@ -9058,7 +9265,7 @@
         <v>1</v>
       </c>
       <c r="I54" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>27</v>
@@ -9067,7 +9274,7 @@
         <v>27</v>
       </c>
       <c r="L54" s="6">
-        <v>0.37435066699981601</v>
+        <v>0.27639716863632202</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
@@ -9075,28 +9282,28 @@
         <v>13</v>
       </c>
       <c r="B55" s="6">
-        <v>14156.2275903224</v>
+        <v>16774.936676502199</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>207</v>
+        <v>307</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>208</v>
+        <v>329</v>
       </c>
       <c r="E55" s="6">
-        <v>5.2500000000000003E-3</v>
+        <v>6.6499999999999997E-3</v>
       </c>
       <c r="F55" s="1">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G55" s="1">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H55" s="1">
-        <v>0</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <v>10</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>27</v>
@@ -9105,7 +9312,7 @@
         <v>27</v>
       </c>
       <c r="L55" s="6">
-        <v>0.36956906318664501</v>
+        <v>0.27613264322280801</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
@@ -9113,37 +9320,37 @@
         <v>16</v>
       </c>
       <c r="B56" s="6">
-        <v>6867.1683101653998</v>
+        <v>15058.0399210453</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>186</v>
+        <v>337</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>229</v>
+        <v>338</v>
       </c>
       <c r="E56" s="6">
-        <v>8.8999999999999999E-3</v>
+        <v>6.8500000000000002E-3</v>
       </c>
       <c r="F56" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G56" s="1">
+        <v>10</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1">
         <v>55</v>
       </c>
-      <c r="H56" s="1">
-        <v>1</v>
-      </c>
-      <c r="I56" s="1">
-        <v>10</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>27</v>
+      <c r="J56" s="1">
+        <v>45</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L56" s="6">
-        <v>0.37933316826820301</v>
+        <v>0.27653184533119202</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
@@ -9151,28 +9358,28 @@
         <v>19</v>
       </c>
       <c r="B57" s="6">
-        <v>14633.7433166503</v>
+        <v>30965.903075456601</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>250</v>
+        <v>347</v>
       </c>
       <c r="E57" s="6">
-        <v>1.9499999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="F57" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G57" s="1">
         <v>60</v>
       </c>
       <c r="H57" s="1">
-        <v>0</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="I57" s="1">
+        <v>55</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>27</v>
@@ -9181,7 +9388,7 @@
         <v>27</v>
       </c>
       <c r="L57" s="6">
-        <v>0.36918982863426197</v>
+        <v>0.27631285786628701</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
@@ -9189,37 +9396,37 @@
         <v>22</v>
       </c>
       <c r="B58" s="6">
-        <v>10873.909991025899</v>
+        <v>29043.666445970499</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>269</v>
+        <v>352</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>270</v>
+        <v>353</v>
       </c>
       <c r="E58" s="6">
-        <v>4.4999999999999997E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="F58" s="1">
+        <v>55</v>
+      </c>
+      <c r="G58" s="1">
+        <v>50</v>
+      </c>
+      <c r="H58" s="1">
+        <v>2</v>
+      </c>
+      <c r="I58" s="1">
         <v>35</v>
       </c>
-      <c r="G58" s="1">
-        <v>45</v>
-      </c>
-      <c r="H58" s="1">
-        <v>0</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>27</v>
+      <c r="J58" s="1">
+        <v>35</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>27</v>
       </c>
       <c r="L58" s="6">
-        <v>0.37450879812240601</v>
+        <v>0.27599468827247597</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
@@ -9227,37 +9434,37 @@
         <v>25</v>
       </c>
       <c r="B59" s="6">
-        <v>11960.240123510301</v>
+        <v>21771.761859893799</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>22</v>
+        <v>359</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>288</v>
+        <v>360</v>
       </c>
       <c r="E59" s="6">
-        <v>3.3999999999999998E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="F59" s="1">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G59" s="1">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H59" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I59" s="1">
-        <v>60</v>
-      </c>
-      <c r="J59" s="1">
-        <v>55</v>
-      </c>
-      <c r="K59" s="1">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="L59" s="6">
-        <v>0.377316445112228</v>
+        <v>0.27616298198699901</v>
       </c>
     </row>
   </sheetData>
@@ -9658,7 +9865,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DD1869-AF27-465D-B713-C899C2D1936F}">
-  <dimension ref="A2:B47"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -9669,378 +9876,374 @@
     <col min="1" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>255</v>
+      <c r="A3" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>250</v>
+      <c r="A4" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>220</v>
+        <v>352</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>221</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>236</v>
+        <v>356</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>237</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>245</v>
+        <v>343</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>246</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>269</v>
+        <v>343</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>278</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>269</v>
+        <v>337</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>274</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>284</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>208</v>
+      <c r="A12" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>262</v>
+      <c r="A13" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>258</v>
+      <c r="A14" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>233</v>
+      <c r="A15" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>212</v>
+      <c r="A16" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>199</v>
+      <c r="A17" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>288</v>
+      <c r="A18" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>266</v>
+      <c r="A19" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>225</v>
+        <v>307</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>226</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>192</v>
+      <c r="A21" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>173</v>
+        <v>313</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>177</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>174</v>
+      <c r="A23" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>269</v>
+        <v>307</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>270</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>229</v>
+      <c r="A25" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>241</v>
+      <c r="A26" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>216</v>
+      <c r="A27" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>159</v>
+      <c r="A28" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>196</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>169</v>
+      <c r="A30" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>151</v>
+        <v>313</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>187</v>
+      <c r="A32" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>181</v>
+        <v>313</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>128</v>
+      <c r="A34" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>151</v>
+        <v>313</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>155</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>146</v>
+        <v>345</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>147</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>108</v>
+      <c r="A37" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>202</v>
+        <v>310</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>203</v>
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>119</v>
+      <c r="A39" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>164</v>
+      <c r="A40" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>310</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>133</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>137</v>
+        <v>304</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>143</v>
+      <c r="A43" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>112</v>
+        <v>304</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>124</v>
+      <c r="A45" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>27</v>
+      <c r="A46" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B47" xr:uid="{07DD1869-AF27-465D-B713-C899C2D1936F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B47">
-      <sortCondition descending="1" ref="B2:B47"/>
+  <autoFilter ref="A2:B2" xr:uid="{07DD1869-AF27-465D-B713-C899C2D1936F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B46">
+      <sortCondition descending="1" ref="B2"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>